<commit_message>
Ignore erroneous spaces in excel fields when converting to JSON
</commit_message>
<xml_diff>
--- a/assay_data/NGARD/NGARD_assays.xlsx
+++ b/assay_data/NGARD/NGARD_assays.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2300" windowWidth="38400" windowHeight="24000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="4300" yWindow="2300" windowWidth="38400" windowHeight="24000" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="All_Assays" sheetId="1" r:id="rId1"/>
     <sheet name="NGARDv1511" sheetId="4" r:id="rId2"/>
     <sheet name="NGARDv1601" sheetId="5" r:id="rId3"/>
     <sheet name="Ecoli" sheetId="6" r:id="rId4"/>
+    <sheet name="Staph" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4972" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5220" uniqueCount="902">
   <si>
     <t>Assay Name</t>
   </si>
@@ -2909,12 +2910,53 @@
   <si>
     <t>references/tuf_UT2_reference.fasta</t>
   </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Positions</t>
+  </si>
+  <si>
+    <r>
+      <t>AA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/NT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Sequence</t>
+    </r>
+  </si>
+  <si>
+    <t>Resistance</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3012,7 +3054,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -3133,593 +3175,631 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="564">
+  <cellStyleXfs count="569">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
@@ -3734,11 +3814,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="50" applyFont="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -3749,7 +3829,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3766,40 +3846,56 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="50" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="564">
+  <cellStyles count="569">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -4342,6 +4438,11 @@
     <cellStyle name="Followed Hyperlink" xfId="561" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="563" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="565" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="567" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -14386,8 +14487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="N177" sqref="N177"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A157" sqref="A157:XFD157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -22376,4 +22477,947 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" s="1" customFormat="1">
+      <c r="A1" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="40"/>
+      <c r="J1" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="45"/>
+      <c r="AB1" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC1" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD1" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE1" s="36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" s="1" customFormat="1" ht="16" thickBot="1">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="46" t="s">
+        <v>898</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>898</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>900</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="R2" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="48" t="s">
+        <v>901</v>
+      </c>
+      <c r="AB2" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC2" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD2" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE2" s="36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="16" thickTop="1">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" s="37"/>
+      <c r="R3" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31">
+      <c r="A4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>356</v>
+      </c>
+      <c r="H4" t="s">
+        <v>365</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="J4" s="37"/>
+      <c r="R4" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31">
+      <c r="H5" t="s">
+        <v>366</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="J5" s="37"/>
+      <c r="R5" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
+      <c r="H6" t="s">
+        <v>367</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="J6" s="37"/>
+      <c r="R6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31">
+      <c r="H7" t="s">
+        <v>368</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="J7" s="37"/>
+      <c r="R7" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31">
+      <c r="H8" t="s">
+        <v>369</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="J8" s="37"/>
+      <c r="R8" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31">
+      <c r="A9" t="s">
+        <v>363</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>364</v>
+      </c>
+      <c r="H9" t="s">
+        <v>370</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="J9" s="37"/>
+      <c r="R9" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31">
+      <c r="A10" t="s">
+        <v>473</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>483</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="J10" s="37"/>
+      <c r="R10" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31">
+      <c r="A11" t="s">
+        <v>474</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>483</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="J11" s="37"/>
+      <c r="R11" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31">
+      <c r="A12" t="s">
+        <v>475</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>483</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="J12" s="37"/>
+      <c r="R12" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31">
+      <c r="A13" t="s">
+        <v>476</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>483</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="J13" s="37"/>
+      <c r="R13" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31">
+      <c r="A14" t="s">
+        <v>477</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>483</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="J14" s="37"/>
+      <c r="R14" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31">
+      <c r="A15" t="s">
+        <v>478</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>483</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="J15" s="37"/>
+      <c r="R15" s="14" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31">
+      <c r="A16" t="s">
+        <v>479</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>483</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="J16" s="37"/>
+      <c r="R16" s="14" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="A17" t="s">
+        <v>480</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>483</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="J17" s="37"/>
+      <c r="R17" s="14" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" t="s">
+        <v>481</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
+        <v>483</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="J18" s="37"/>
+      <c r="R18" s="14" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" t="s">
+        <v>482</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>483</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="J19" s="37"/>
+      <c r="R19" s="14" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" t="s">
+        <v>386</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
+        <v>395</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="J20" s="37"/>
+      <c r="K20">
+        <v>30</v>
+      </c>
+      <c r="L20" t="s">
+        <v>399</v>
+      </c>
+      <c r="M20" t="s">
+        <v>398</v>
+      </c>
+      <c r="R20" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" t="s">
+        <v>381</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
+        <v>394</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="J21" s="37"/>
+      <c r="K21">
+        <v>37</v>
+      </c>
+      <c r="L21" t="s">
+        <v>398</v>
+      </c>
+      <c r="M21" t="s">
+        <v>399</v>
+      </c>
+      <c r="R21" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" t="s">
+        <v>795</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>794</v>
+      </c>
+      <c r="J22" s="37"/>
+      <c r="K22">
+        <v>46</v>
+      </c>
+      <c r="L22" t="s">
+        <v>399</v>
+      </c>
+      <c r="M22" t="s">
+        <v>398</v>
+      </c>
+      <c r="R22" t="s">
+        <v>796</v>
+      </c>
+      <c r="S22" s="1"/>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23" t="s">
+        <v>385</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="J23" s="37"/>
+      <c r="K23">
+        <v>33</v>
+      </c>
+      <c r="L23" t="s">
+        <v>398</v>
+      </c>
+      <c r="M23" t="s">
+        <v>399</v>
+      </c>
+      <c r="R23" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24" t="s">
+        <v>383</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="J24" s="37"/>
+      <c r="K24">
+        <v>39</v>
+      </c>
+      <c r="L24" t="s">
+        <v>398</v>
+      </c>
+      <c r="M24" t="s">
+        <v>399</v>
+      </c>
+      <c r="R24" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" t="s">
+        <v>384</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="J25" s="37"/>
+      <c r="K25">
+        <v>58</v>
+      </c>
+      <c r="L25" t="s">
+        <v>399</v>
+      </c>
+      <c r="M25" t="s">
+        <v>398</v>
+      </c>
+      <c r="R25" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" t="s">
+        <v>382</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="J26" s="37"/>
+      <c r="K26">
+        <v>44</v>
+      </c>
+      <c r="L26" t="s">
+        <v>398</v>
+      </c>
+      <c r="M26" t="s">
+        <v>399</v>
+      </c>
+      <c r="R26" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27" t="s">
+        <v>790</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" s="26" t="s">
+        <v>792</v>
+      </c>
+      <c r="J27" s="49"/>
+      <c r="K27">
+        <v>56</v>
+      </c>
+      <c r="L27" t="s">
+        <v>397</v>
+      </c>
+      <c r="M27" t="s">
+        <v>398</v>
+      </c>
+      <c r="R27" t="s">
+        <v>517</v>
+      </c>
+      <c r="S27" s="1"/>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" t="s">
+        <v>791</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="I28" s="26" t="s">
+        <v>793</v>
+      </c>
+      <c r="J28" s="49"/>
+      <c r="K28">
+        <v>46</v>
+      </c>
+      <c r="L28" t="s">
+        <v>399</v>
+      </c>
+      <c r="M28" t="s">
+        <v>398</v>
+      </c>
+      <c r="R28" t="s">
+        <v>517</v>
+      </c>
+      <c r="S28" s="1"/>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29" t="s">
+        <v>400</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>402</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="J29" s="37"/>
+      <c r="R29" s="17" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" t="s">
+        <v>401</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" t="s">
+        <v>403</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="J30" s="37"/>
+      <c r="R30" s="17" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" t="s">
+        <v>324</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" t="s">
+        <v>334</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="P31" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32" t="s">
+        <v>164</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" t="s">
+        <v>177</v>
+      </c>
+      <c r="G32" t="s">
+        <v>472</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="M32" t="s">
+        <v>198</v>
+      </c>
+      <c r="N32" t="s">
+        <v>199</v>
+      </c>
+      <c r="O32" t="s">
+        <v>322</v>
+      </c>
+      <c r="P32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" t="s">
+        <v>176</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>178</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="M33" t="s">
+        <v>560</v>
+      </c>
+      <c r="N33" t="s">
+        <v>212</v>
+      </c>
+      <c r="O33" t="s">
+        <v>322</v>
+      </c>
+      <c r="P33" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" t="s">
+        <v>325</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" t="s">
+        <v>335</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="P34" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" t="s">
+        <v>316</v>
+      </c>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" t="s">
+        <v>314</v>
+      </c>
+      <c r="G35" t="s">
+        <v>472</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="M35" t="s">
+        <v>470</v>
+      </c>
+      <c r="N35" t="s">
+        <v>319</v>
+      </c>
+      <c r="O35" t="s">
+        <v>320</v>
+      </c>
+      <c r="P35" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="G36" t="s">
+        <v>472</v>
+      </c>
+      <c r="I36" s="9"/>
+      <c r="M36" t="s">
+        <v>471</v>
+      </c>
+      <c r="N36" t="s">
+        <v>469</v>
+      </c>
+      <c r="O36" t="s">
+        <v>468</v>
+      </c>
+      <c r="P36" t="s">
+        <v>317</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+  </mergeCells>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C27:C28 C22">
+      <formula1>$AC$1:$AC$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27:B28 B22">
+      <formula1>$AB$1:$AB$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C23:C26 C29:C30 C9:C21 C3:C4">
+      <formula1>$AC$1:$AC$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B26 B29:B30 B9:B21 B3:B4">
+      <formula1>$AB$1:$AB$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31:B35">
+      <formula1>$AB$1:$AB$21</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C31:C35">
+      <formula1>$AC$1:$AC$21</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>